<commit_message>
Refactored Tutor initialisation - can't defer LoadStudents()/LoadWorld()/LoadDomain() method calls
</commit_message>
<xml_diff>
--- a/DomainConf/Tutorial.xlsx
+++ b/DomainConf/Tutorial.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Diego/Documents/workspace/ITS/DomainConf/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="20740" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ConfTutorial" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>1-Debe sentarse antes de tomar el café.</t>
   </si>
@@ -219,6 +214,9 @@
   </si>
   <si>
     <t>DentroDelPlan</t>
+  </si>
+  <si>
+    <t>1-Something something</t>
   </si>
 </sst>
 </file>
@@ -310,18 +308,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -658,16 +656,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="16384" width="17.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" ht="12.75" customHeight="1">
       <c r="C1" s="1" t="s">
         <v>53</v>
       </c>
@@ -729,7 +727,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" ht="12.75" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -772,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" ht="12.75" customHeight="1">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -829,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" ht="12.75" customHeight="1">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -877,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" ht="12.75" customHeight="1">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -925,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" ht="12.75" customHeight="1">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -973,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" ht="12.75" customHeight="1">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1021,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" ht="12.75" customHeight="1">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1033,6 +1031,9 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="F8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1066,7 +1067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" ht="12.75" customHeight="1">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -1113,630 +1114,630 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" ht="12.75" customHeight="1">
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="I10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:22" ht="12.75" customHeight="1">
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="I11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" ht="12.75" customHeight="1">
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="I12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" ht="12.75" customHeight="1">
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="I13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" ht="12.75" customHeight="1">
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="I14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" ht="12.75" customHeight="1">
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="I15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" ht="12.75" customHeight="1">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="I16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="5:12" ht="12.75" customHeight="1">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="I17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="5:12" ht="12.75" customHeight="1">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="I18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="5:12" ht="12.75" customHeight="1">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="I19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="5:12" ht="12.75" customHeight="1">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="5:12" ht="12.75" customHeight="1">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="I21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="5:12" ht="12.75" customHeight="1">
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="I22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="5:12" ht="12.75" customHeight="1">
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="I23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="5:12" ht="12.75" customHeight="1">
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="I24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="5:12" ht="12.75" customHeight="1">
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="I25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="5:12" ht="12.75" customHeight="1">
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="I26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="5:12" ht="12.75" customHeight="1">
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="I27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="5:12" ht="12.75" customHeight="1">
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="I28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="5:12" ht="12.75" customHeight="1">
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="I29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="5:12" ht="12.75" customHeight="1">
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="I30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="5:12" ht="12.75" customHeight="1">
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="I31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="5:12" ht="12.75" customHeight="1">
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="I32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="5:12" ht="12.75" customHeight="1">
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="I33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="5:12" ht="12.75" customHeight="1">
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="I34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="5:12" ht="12.75" customHeight="1">
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="I35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="5:12" ht="12.75" customHeight="1">
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="I36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="5:12" ht="12.75" customHeight="1">
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="I37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="5:12" ht="12.75" customHeight="1">
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="I38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="5:12" ht="12.75" customHeight="1">
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="I39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="5:12" ht="12.75" customHeight="1">
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="I40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="5:12" ht="12.75" customHeight="1">
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="I41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="5:12" ht="12.75" customHeight="1">
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="I42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="5:12" ht="12.75" customHeight="1">
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="I43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="5:12" ht="12.75" customHeight="1">
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="I44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="5:12" ht="12.75" customHeight="1">
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="I45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="5:12" ht="12.75" customHeight="1">
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="I46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="5:12" ht="12.75" customHeight="1">
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="I47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="5:12" ht="12.75" customHeight="1">
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="I48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="5:12" ht="12.75" customHeight="1">
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="I49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="5:12" ht="12.75" customHeight="1">
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="I50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="5:12" ht="12.75" customHeight="1">
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="I51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="5:12" ht="12.75" customHeight="1">
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="I52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="5:12" ht="12.75" customHeight="1">
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="I53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="5:12" ht="12.75" customHeight="1">
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="I54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="5:12" ht="12.75" customHeight="1">
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="I55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="5:12" ht="12.75" customHeight="1">
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="I56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="5:12" ht="12.75" customHeight="1">
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="I57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="5:12" ht="12.75" customHeight="1">
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="I58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="5:12" ht="12.75" customHeight="1">
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="I59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="5:12" ht="12.75" customHeight="1">
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="I60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="5:12" ht="12.75" customHeight="1">
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="I61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="5:12" ht="12.75" customHeight="1">
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="I62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="5:12" ht="12.75" customHeight="1">
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="I63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="5:12" ht="12.75" customHeight="1">
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="I64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="5:12" ht="12.75" customHeight="1">
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="I65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="5:12" ht="12.75" customHeight="1">
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="I66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="5:12" ht="12.75" customHeight="1">
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="I67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="5:12" ht="12.75" customHeight="1">
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="I68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="5:12" ht="12.75" customHeight="1">
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="I69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="5:12" ht="12.75" customHeight="1">
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="I70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="5:12" ht="12.75" customHeight="1">
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="I71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="5:12" ht="12.75" customHeight="1">
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="I72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="5:12" ht="12.75" customHeight="1">
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="I73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="5:12" ht="12.75" customHeight="1">
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="I74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="5:12" ht="12.75" customHeight="1">
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="I75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="5:12" ht="12.75" customHeight="1">
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="I76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="5:12" ht="12.75" customHeight="1">
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="I77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="5:12" ht="12.75" customHeight="1">
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="I78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="5:12" ht="12.75" customHeight="1">
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="I79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="5:12" ht="12.75" customHeight="1">
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="I80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="5:12" ht="12.75" customHeight="1">
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="I81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="5:12" ht="12.75" customHeight="1">
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="I82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="5:12" ht="12.75" customHeight="1">
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="I83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="5:12" ht="12.75" customHeight="1">
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
       <c r="I84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="5:12" ht="12.75" customHeight="1">
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="I85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="5:12" ht="12.75" customHeight="1">
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="I86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="5:12" ht="12.75" customHeight="1">
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="I87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="5:12" ht="12.75" customHeight="1">
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="I88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="5:12" ht="12.75" customHeight="1">
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="I89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="5:12" ht="12.75" customHeight="1">
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
       <c r="I90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="5:12" ht="12.75" customHeight="1">
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
       <c r="I91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="5:12" ht="12.75" customHeight="1">
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
       <c r="I92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="5:12" ht="12.75" customHeight="1">
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
       <c r="I93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="5:12" ht="12.75" customHeight="1">
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="I94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="5:12" ht="12.75" customHeight="1">
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="I95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="5:12" ht="12.75" customHeight="1">
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="I96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="5:12" ht="12.75" customHeight="1">
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="I97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="5:12" ht="12.75" customHeight="1">
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="I98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="5:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="5:12" ht="12.75" customHeight="1">
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -1745,6 +1746,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Configuring Collective Model action support threshold individually for each of the actions in spreadsheet
</commit_message>
<xml_diff>
--- a/DomainConf/Tutorial.xlsx
+++ b/DomainConf/Tutorial.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>1-Debe sentarse antes de tomar el café.</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>1-Something something</t>
+  </si>
+  <si>
+    <t>Is Checkpoint?</t>
+  </si>
+  <si>
+    <t>Collective Student Model Tutor messages</t>
+  </si>
+  <si>
+    <t>Support Threshold</t>
   </si>
 </sst>
 </file>
@@ -277,8 +286,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -307,19 +318,21 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -654,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V99"/>
+  <dimension ref="A1:Y99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -665,7 +678,7 @@
     <col min="1" max="16384" width="17.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="12.75" customHeight="1">
+    <row r="1" spans="1:25" ht="12.75" customHeight="1">
       <c r="C1" s="1" t="s">
         <v>53</v>
       </c>
@@ -726,8 +739,17 @@
       <c r="V1" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="12.75" customHeight="1">
+      <c r="W1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="12.75" customHeight="1">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -770,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="12.75" customHeight="1">
+    <row r="3" spans="1:25" ht="12.75" customHeight="1">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -827,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="12.75" customHeight="1">
+    <row r="4" spans="1:25" ht="12.75" customHeight="1">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -875,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="12.75" customHeight="1">
+    <row r="5" spans="1:25" ht="12.75" customHeight="1">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -923,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="12.75" customHeight="1">
+    <row r="6" spans="1:25" ht="12.75" customHeight="1">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -971,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="12.75" customHeight="1">
+    <row r="7" spans="1:25" ht="12.75" customHeight="1">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1019,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="12.75" customHeight="1">
+    <row r="8" spans="1:25" ht="12.75" customHeight="1">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1067,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="12.75" customHeight="1">
+    <row r="9" spans="1:25" ht="12.75" customHeight="1">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -1114,49 +1136,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="12.75" customHeight="1">
+    <row r="10" spans="1:25" ht="12.75" customHeight="1">
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="I10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="12.75" customHeight="1">
+    <row r="11" spans="1:25" ht="12.75" customHeight="1">
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="I11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="12.75" customHeight="1">
+    <row r="12" spans="1:25" ht="12.75" customHeight="1">
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="I12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="12.75" customHeight="1">
+    <row r="13" spans="1:25" ht="12.75" customHeight="1">
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="I13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:22" ht="12.75" customHeight="1">
+    <row r="14" spans="1:25" ht="12.75" customHeight="1">
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="I14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="12.75" customHeight="1">
+    <row r="15" spans="1:25" ht="12.75" customHeight="1">
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="I15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:22" ht="12.75" customHeight="1">
+    <row r="16" spans="1:25" ht="12.75" customHeight="1">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1746,6 +1768,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>